<commit_message>
Text box y 2nd dynamic treeview
</commit_message>
<xml_diff>
--- a/Cursos-DB.xlsx
+++ b/Cursos-DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Empleados" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="126">
   <si>
     <t xml:space="preserve">Legajo</t>
   </si>
@@ -263,16 +263,16 @@
     <t xml:space="preserve">Aprobado</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">WBT-HS_E-009</t>
   </si>
   <si>
-    <t xml:space="preserve">Aislamiento de sistemas peligrosos y apertura de lineas por WBT</t>
+    <t xml:space="preserve">Aislamiento de Truestemas peligrosos y apertura de lineas por WBT</t>
   </si>
   <si>
     <t xml:space="preserve">WBT-HS_E-019 BA</t>
@@ -296,13 +296,13 @@
     <t xml:space="preserve">WBT-HS_E-012-L</t>
   </si>
   <si>
-    <t xml:space="preserve">Ergonomia-Anual</t>
+    <t xml:space="preserve">ErgoFalsemia-Anual</t>
   </si>
   <si>
     <t xml:space="preserve">HS_E-015</t>
   </si>
   <si>
-    <t xml:space="preserve">Manejo y Disposición de Residuos Solidos</t>
+    <t xml:space="preserve">Manejo y DispoTrueción de ReTrueduos Solidos</t>
   </si>
   <si>
     <t xml:space="preserve">WBT-HS_E-001-L</t>
@@ -320,7 +320,7 @@
     <t xml:space="preserve">SOP-HS_E-013</t>
   </si>
   <si>
-    <t xml:space="preserve">Manejo Interno de residuos</t>
+    <t xml:space="preserve">Manejo InterFalse de reTrueduos</t>
   </si>
   <si>
     <t xml:space="preserve">SOP-HS_E-048</t>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">WBT-HS_E-014</t>
   </si>
   <si>
-    <t xml:space="preserve">BEST-Entrenamiento basico de segruridad electrica</t>
+    <t xml:space="preserve">BEST-Entrenamiento baTrueco de segruridad electrica</t>
   </si>
   <si>
     <t xml:space="preserve">ID-Evento</t>
@@ -399,9 +399,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cursos       Lineas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">Mecánico</t>
@@ -418,7 +415,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -440,14 +437,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -492,8 +481,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,15 +494,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -661,53 +646,53 @@
     <tabColor rgb="FF375623"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>132</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -716,7 +701,7 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>40654321</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -728,7 +713,7 @@
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -736,7 +721,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>432</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -745,7 +730,7 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>44568987</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -762,7 +747,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>354</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -771,7 +756,7 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>26897654</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -788,7 +773,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>852</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -797,7 +782,7 @@
       <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>37654789</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -814,7 +799,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>684</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -823,7 +808,7 @@
       <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>29195735</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -840,7 +825,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>915</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -849,7 +834,7 @@
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>20345915</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -866,7 +851,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>147</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -875,7 +860,7 @@
       <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>32687459</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -890,6 +875,9 @@
       <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -949,14 +937,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,7 +980,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>20974563</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1004,7 +992,7 @@
       <c r="D2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>132</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1021,7 +1009,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1033,7 +1021,7 @@
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>432</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1050,7 +1038,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>39852147</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1062,7 +1050,7 @@
       <c r="D4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="2"/>
@@ -1070,7 +1058,7 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>43915678</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1082,7 +1070,7 @@
       <c r="D5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>852</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1099,7 +1087,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>28945387</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1111,7 +1099,7 @@
       <c r="D6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>684</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1128,7 +1116,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>35658945</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1140,7 +1128,7 @@
       <c r="D7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="2"/>
@@ -1148,7 +1136,7 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>42357951</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1160,7 +1148,7 @@
       <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>147</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1236,32 +1224,32 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="23" style="0" width="4.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="23" style="1" width="5.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,75 +1283,75 @@
       <c r="J1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="W1" s="0" t="n">
+      <c r="W1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="X1" s="0" t="n">
+      <c r="X1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Y1" s="0" t="n">
+      <c r="Y1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Z1" s="0" t="n">
+      <c r="Z1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>42357951</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -1416,25 +1404,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>39852147</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>20974563</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -1487,25 +1475,25 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>43915678</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>20974563</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1558,25 +1546,25 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1629,25 +1617,25 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>42357951</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>28945387</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1700,25 +1688,25 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>20974563</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1771,25 +1759,25 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>20974563</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>35658945</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1842,25 +1830,25 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1913,25 +1901,25 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>28945387</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>35658945</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1984,25 +1972,25 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>42357951</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -2055,25 +2043,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>35658945</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>42357951</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -2126,25 +2114,25 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>42357951</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>20974563</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -2197,25 +2185,25 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>42357951</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>20974563</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -2268,25 +2256,25 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>20974563</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2339,25 +2327,25 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>20974563</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>28945387</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -2410,25 +2398,25 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -2481,25 +2469,25 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>28945387</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>39852147</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -2552,25 +2540,25 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>38963856</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>43915678</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -2623,25 +2611,25 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>39852147</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>38963856</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -2694,25 +2682,25 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>43915678</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>42357951</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -2805,34 +2793,34 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="17.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C2" s="3" t="n">
@@ -2840,10 +2828,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C3" s="3" t="n">
@@ -2851,10 +2839,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="3" t="n">
@@ -2862,10 +2850,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -2873,10 +2861,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -2884,10 +2872,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="3" t="n">
@@ -2895,10 +2883,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -2906,10 +2894,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="3" t="n">
@@ -2917,10 +2905,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="3" t="n">
@@ -2928,10 +2916,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C11" s="3" t="n">
@@ -2939,10 +2927,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C12" s="3" t="n">
@@ -2950,10 +2938,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C13" s="3" t="n">
@@ -2961,10 +2949,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="3" t="n">
@@ -2972,10 +2960,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C15" s="3" t="n">
@@ -2983,10 +2971,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C16" s="3" t="n">
@@ -2994,10 +2982,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C17" s="3" t="n">
@@ -3005,10 +2993,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C18" s="3" t="n">
@@ -3016,10 +3004,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C19" s="3" t="n">
@@ -3027,10 +3015,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C20" s="3" t="n">
@@ -3038,10 +3026,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C21" s="3" t="n">
@@ -3068,38 +3056,38 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3119,7 +3107,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3139,7 +3127,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3159,7 +3147,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3179,7 +3167,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3199,7 +3187,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3219,7 +3207,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3239,7 +3227,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3259,7 +3247,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3279,7 +3267,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3299,7 +3287,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3319,7 +3307,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3339,7 +3327,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3359,7 +3347,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3379,7 +3367,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3399,7 +3387,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3419,7 +3407,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3439,7 +3427,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3459,7 +3447,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3479,7 +3467,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -3524,49 +3512,49 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3592,7 +3580,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3618,7 +3606,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3644,7 +3632,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3670,7 +3658,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3696,7 +3684,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3722,7 +3710,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3748,7 +3736,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3774,7 +3762,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3800,7 +3788,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3826,7 +3814,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3852,7 +3840,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3878,7 +3866,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3904,7 +3892,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -3930,7 +3918,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3956,7 +3944,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -3982,7 +3970,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -4008,7 +3996,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -4034,7 +4022,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -4060,7 +4048,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4111,34 +4099,34 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="D1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4155,7 +4143,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4172,7 +4160,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4189,7 +4177,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4206,7 +4194,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4223,7 +4211,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -4240,7 +4228,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4257,7 +4245,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4274,7 +4262,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4291,7 +4279,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4308,7 +4296,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -4325,7 +4313,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -4342,7 +4330,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -4359,7 +4347,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4376,7 +4364,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4393,7 +4381,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -4410,7 +4398,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -4427,7 +4415,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -4444,7 +4432,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -4461,7 +4449,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4502,18 +4490,18 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,7 +4514,7 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -4542,156 +4530,156 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>